<commit_message>
Merged in feature/Add_Authentication (pull request #3)
Feature/Add JWT Authentication and User login/Registration Endpoints

* Add JWT Authentication and User login/Registeration Endpoints


Approved-by: Wael Yassir
</commit_message>
<xml_diff>
--- a/_Docs/Features.xlsx
+++ b/_Docs/Features.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ya4\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bary\source\repos\VCProjectGallery\_Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:0_{21480240-6398-4AB8-A121-C8D90BF32DB2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBCC03E3-ABB7-44AC-9282-A84CDA0998D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{C4DE301E-37E4-45AA-AC65-E1505B480707}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{C4DE301E-37E4-45AA-AC65-E1505B480707}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Main Feature</t>
   </si>
@@ -48,16 +48,22 @@
     <t>Webhost (Azure)</t>
   </si>
   <si>
-    <t>Resources Management</t>
-  </si>
-  <si>
-    <t>DB Deployment</t>
-  </si>
-  <si>
     <t>Pipeline</t>
   </si>
   <si>
     <t>Identity</t>
+  </si>
+  <si>
+    <t>DB Deployment [Local]</t>
+  </si>
+  <si>
+    <t>Resources Management [Blob Storage Local]</t>
+  </si>
+  <si>
+    <t>DB Deployment [Cloud]</t>
+  </si>
+  <si>
+    <t>Resources Management [Blob Storage Cloud]</t>
   </si>
 </sst>
 </file>
@@ -73,12 +79,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -93,8 +105,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,70 +422,86 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64BB4D03-53BD-4D91-BE59-76B018699DEC}">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>